<commit_message>
updated template for test case
</commit_message>
<xml_diff>
--- a/api/v1/lib/Oxzion/test/TemplateTest/Data/exportedtemplate1.xlsx
+++ b/api/v1/lib/Oxzion/test/TemplateTest/Data/exportedtemplate1.xlsx
@@ -25,25 +25,25 @@
     <t xml:space="preserve">First name:</t>
   </si>
   <si>
-    <t xml:space="preserve">firstname</t>
+    <t xml:space="preserve">{firstname}</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly expenditure:</t>
   </si>
   <si>
-    <t xml:space="preserve">expenses</t>
+    <t xml:space="preserve">{{expenses}}</t>
   </si>
   <si>
     <t xml:space="preserve">Address: </t>
   </si>
   <si>
-    <t xml:space="preserve">address</t>
+    <t xml:space="preserve">{{address}}</t>
   </si>
   <si>
     <t xml:space="preserve">Hobbies: </t>
   </si>
   <si>
-    <t xml:space="preserve">hobbies</t>
+    <t xml:space="preserve">{{hobbies}}</t>
   </si>
 </sst>
 </file>
@@ -158,7 +158,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1:G1"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>